<commit_message>
add log of kilosort data summary
</commit_message>
<xml_diff>
--- a/doc/UpdateTaskKilosortSummary.xlsx
+++ b/doc/UpdateTaskKilosortSummary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>total recording sessions from 3 mice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maybe a little more unstable than usual? </t>
+  </si>
+  <si>
+    <t>3 clusters were exluded during post-curation</t>
+  </si>
+  <si>
+    <t>a lot of the clusters were noise/purely contamination</t>
   </si>
 </sst>
 </file>
@@ -264,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,7 +289,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -598,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -608,11 +616,11 @@
     <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="18.125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="20.125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="19.125" customWidth="1"/>
+    <col min="9" max="9" width="18.125" customWidth="1"/>
+    <col min="10" max="10" width="20.125" customWidth="1"/>
     <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="79.125" bestFit="1" customWidth="1"/>
@@ -857,41 +865,45 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
         <v>17</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>210409</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
         <v>51</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="L7" s="3">
+        <v>26</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -951,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -1457,41 +1469,43 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="5">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3">
         <v>20</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>210511</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="5">
-        <v>1</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1</v>
-      </c>
-      <c r="H23" s="5">
-        <v>1</v>
-      </c>
-      <c r="I23" s="5">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3">
         <v>78</v>
       </c>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="L23" s="3">
+        <v>33</v>
+      </c>
+      <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1533,41 +1547,45 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="5">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3">
         <v>20</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="3">
         <v>210512</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5">
-        <v>1</v>
-      </c>
-      <c r="G25" s="5">
-        <v>1</v>
-      </c>
-      <c r="H25" s="5">
-        <v>1</v>
-      </c>
-      <c r="I25" s="5">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0</v>
-      </c>
-      <c r="K25" s="5">
+      <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>1</v>
+      </c>
+      <c r="K25" s="3">
         <v>94</v>
       </c>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="L25" s="3">
+        <v>49</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1845,7 +1863,7 @@
       <c r="M32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N32" s="14">
+      <c r="N32" s="13">
         <v>12</v>
       </c>
       <c r="O32" t="s">
@@ -1931,7 +1949,7 @@
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="14">
+      <c r="N34" s="13">
         <v>30</v>
       </c>
       <c r="O34" t="s">
@@ -2659,41 +2677,45 @@
       <c r="M52" s="5"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="5">
+      <c r="A53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="3">
         <v>25</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="12">
         <v>210912</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="5">
-        <v>1</v>
-      </c>
-      <c r="F53" s="5">
-        <v>0</v>
-      </c>
-      <c r="G53" s="5">
-        <v>0</v>
-      </c>
-      <c r="H53" s="5">
-        <v>0</v>
-      </c>
-      <c r="I53" s="5">
-        <v>0</v>
-      </c>
-      <c r="J53" s="5">
-        <v>0</v>
-      </c>
-      <c r="K53" s="5">
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3">
+        <v>1</v>
+      </c>
+      <c r="I53" s="3">
+        <v>1</v>
+      </c>
+      <c r="J53" s="3">
+        <v>1</v>
+      </c>
+      <c r="K53" s="3">
         <v>52</v>
       </c>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
+      <c r="L53" s="3">
+        <v>42</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
@@ -2737,43 +2759,43 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="4">
+      <c r="A55" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="3">
         <v>25</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="12">
         <v>210913</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="4">
-        <v>1</v>
-      </c>
-      <c r="F55" s="4">
-        <v>1</v>
-      </c>
-      <c r="G55" s="4">
-        <v>1</v>
-      </c>
-      <c r="H55" s="4">
-        <v>1</v>
-      </c>
-      <c r="I55" s="4">
-        <v>1</v>
-      </c>
-      <c r="J55" s="4">
-        <v>0</v>
-      </c>
-      <c r="K55" s="4">
+      <c r="D55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="3">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
         <v>79</v>
       </c>
-      <c r="L55" s="4">
+      <c r="L55" s="3">
         <v>55</v>
       </c>
-      <c r="M55" s="4"/>
+      <c r="M55" s="3"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">

</xml_diff>